<commit_message>
change 'ignoreEmptyLines' to be default 'true'
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjacob101/git/github.com/bradjacobs/excel-to-csv/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradjacobs/git/bradjacobs/excel-to-csv/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6D967E-A8CF-374F-B7D6-489B9234D3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311DEEFF-1ACB-9043-8A91-480EDA47635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="4580" windowWidth="26440" windowHeight="15440" xr2:uid="{1C8AC41B-F10E-D845-B5C5-16AC4F1A1759}"/>
+    <workbookView xWindow="2360" yWindow="1540" windowWidth="26440" windowHeight="15440" xr2:uid="{1C8AC41B-F10E-D845-B5C5-16AC4F1A1759}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_SHEET" sheetId="1" r:id="rId1"/>
+    <sheet name="TEST_BLANK_SHEET" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -483,9 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB26578-327A-6945-AB21-86CB10BF1AB3}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -647,4 +646,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D4D85C-ED89-2F4D-BC5E-B2BB98AC7BF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>